<commit_message>
Update Datapath Control Sheet
</commit_message>
<xml_diff>
--- a/Datapath_Control_Sheet.xlsx
+++ b/Datapath_Control_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Project\iverilog\Exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B59DA3-2E5B-4EA5-9A6B-8B72782FA4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE605B31-6CC1-451B-B0F2-7FE2DB189768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据通路表(含控制信号)" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="178">
   <si>
     <t>所属单元</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -569,19 +569,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BrUnSel</t>
-  </si>
-  <si>
-    <t>BrUnSel_Non(3'b0)</t>
-  </si>
-  <si>
-    <t>BrUnSel_Non</t>
-  </si>
-  <si>
-    <t>BrUnSel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MemW_Non(1'b0)</t>
   </si>
   <si>
@@ -653,26 +640,6 @@
   </si>
   <si>
     <t>ImmSel_SB(3'b11)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BrUn_En(1'b1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BrUnSel_Beq(3'b1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BrUnSel_Bne(3'b10)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BrUnSel_Blt(3'b11)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BrUnSel_Bge(3'b100)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -746,6 +713,31 @@
     <t>A&lt;B?
 BrLT_T:BrLT_F</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BrSel</t>
+  </si>
+  <si>
+    <t>BrSel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BrSel_Non(3'b0)</t>
+  </si>
+  <si>
+    <t>BrSel_Non</t>
+  </si>
+  <si>
+    <t>BrSel_Beq(3'b1)</t>
+  </si>
+  <si>
+    <t>BrSel_Bne(3'b10)</t>
+  </si>
+  <si>
+    <t>BrSel_Blt(3'b11)</t>
+  </si>
+  <si>
+    <t>BrSel_Bge(3'b100)</t>
   </si>
 </sst>
 </file>
@@ -912,16 +904,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1243,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1273,30 +1265,30 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="21" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
       <c r="P2" s="22"/>
-      <c r="Q2" s="20" t="s">
+      <c r="Q2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="20"/>
+      <c r="R2" s="23"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1305,35 +1297,35 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
+      <c r="E3" s="23"/>
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21" t="s">
+      <c r="M3" s="23"/>
+      <c r="N3" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="O3" s="23"/>
+      <c r="O3" s="21"/>
       <c r="P3" s="22"/>
-      <c r="Q3" s="20" t="s">
+      <c r="Q3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="20"/>
+      <c r="R3" s="23"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1375,7 +1367,7 @@
       <c r="N4" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="20" t="s">
         <v>78</v>
       </c>
       <c r="P4" s="22"/>
@@ -1420,7 +1412,7 @@
         <v>65</v>
       </c>
       <c r="N5" s="15"/>
-      <c r="O5" s="21"/>
+      <c r="O5" s="20"/>
       <c r="P5" s="22"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="3"/>
@@ -1459,7 +1451,7 @@
         <v>65</v>
       </c>
       <c r="N6" s="15"/>
-      <c r="O6" s="21"/>
+      <c r="O6" s="20"/>
       <c r="P6" s="22"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="3"/>
@@ -1498,7 +1490,7 @@
         <v>64</v>
       </c>
       <c r="N7" s="15"/>
-      <c r="O7" s="21"/>
+      <c r="O7" s="20"/>
       <c r="P7" s="22"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="3"/>
@@ -1537,7 +1529,7 @@
         <v>64</v>
       </c>
       <c r="N8" s="15"/>
-      <c r="O8" s="21"/>
+      <c r="O8" s="20"/>
       <c r="P8" s="22"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="3"/>
@@ -1576,7 +1568,7 @@
         <v>64</v>
       </c>
       <c r="N9" s="15"/>
-      <c r="O9" s="21"/>
+      <c r="O9" s="20"/>
       <c r="P9" s="22"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="3"/>
@@ -1615,7 +1607,7 @@
         <v>64</v>
       </c>
       <c r="N10" s="15"/>
-      <c r="O10" s="21"/>
+      <c r="O10" s="20"/>
       <c r="P10" s="22"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="3"/>
@@ -1654,7 +1646,7 @@
         <v>64</v>
       </c>
       <c r="N11" s="15"/>
-      <c r="O11" s="21"/>
+      <c r="O11" s="20"/>
       <c r="P11" s="22"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="3"/>
@@ -1693,7 +1685,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="15"/>
-      <c r="O12" s="21"/>
+      <c r="O12" s="20"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="3"/>
@@ -1712,7 +1704,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="15"/>
-      <c r="O13" s="21"/>
+      <c r="O13" s="20"/>
       <c r="P13" s="22"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="3"/>
@@ -1751,7 +1743,7 @@
         <v>68</v>
       </c>
       <c r="N14" s="15"/>
-      <c r="O14" s="21"/>
+      <c r="O14" s="20"/>
       <c r="P14" s="22"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="3"/>
@@ -1790,7 +1782,7 @@
         <v>68</v>
       </c>
       <c r="N15" s="15"/>
-      <c r="O15" s="21"/>
+      <c r="O15" s="20"/>
       <c r="P15" s="22"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="3"/>
@@ -1829,7 +1821,7 @@
         <v>68</v>
       </c>
       <c r="N16" s="15"/>
-      <c r="O16" s="21"/>
+      <c r="O16" s="20"/>
       <c r="P16" s="22"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="3"/>
@@ -1868,7 +1860,7 @@
         <v>68</v>
       </c>
       <c r="N17" s="15"/>
-      <c r="O17" s="21"/>
+      <c r="O17" s="20"/>
       <c r="P17" s="22"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="3"/>
@@ -1907,7 +1899,7 @@
         <v>68</v>
       </c>
       <c r="N18" s="15"/>
-      <c r="O18" s="21"/>
+      <c r="O18" s="20"/>
       <c r="P18" s="22"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="3"/>
@@ -1946,7 +1938,7 @@
         <v>68</v>
       </c>
       <c r="N19" s="15"/>
-      <c r="O19" s="21"/>
+      <c r="O19" s="20"/>
       <c r="P19" s="22"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="3"/>
@@ -1985,7 +1977,7 @@
         <v>68</v>
       </c>
       <c r="N20" s="15"/>
-      <c r="O20" s="21"/>
+      <c r="O20" s="20"/>
       <c r="P20" s="22"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="3"/>
@@ -2024,7 +2016,7 @@
         <v>68</v>
       </c>
       <c r="N21" s="15"/>
-      <c r="O21" s="21"/>
+      <c r="O21" s="20"/>
       <c r="P21" s="22"/>
       <c r="Q21" s="6" t="s">
         <v>61</v>
@@ -2067,7 +2059,7 @@
         <v>68</v>
       </c>
       <c r="N22" s="15"/>
-      <c r="O22" s="21"/>
+      <c r="O22" s="20"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="3"/>
@@ -2086,7 +2078,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="15"/>
-      <c r="O23" s="21"/>
+      <c r="O23" s="20"/>
       <c r="P23" s="22"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="3"/>
@@ -2123,7 +2115,7 @@
         <v>68</v>
       </c>
       <c r="N24" s="15"/>
-      <c r="O24" s="21"/>
+      <c r="O24" s="20"/>
       <c r="P24" s="22"/>
       <c r="Q24" s="6" t="s">
         <v>61</v>
@@ -2146,7 +2138,7 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="15"/>
-      <c r="O25" s="21"/>
+      <c r="O25" s="20"/>
       <c r="P25" s="22"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="3"/>
@@ -2187,7 +2179,7 @@
       <c r="N26" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O26" s="21" t="s">
+      <c r="O26" s="20" t="s">
         <v>64</v>
       </c>
       <c r="P26" s="22"/>
@@ -2230,7 +2222,7 @@
       <c r="N27" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O27" s="21" t="s">
+      <c r="O27" s="20" t="s">
         <v>64</v>
       </c>
       <c r="P27" s="22"/>
@@ -2273,7 +2265,7 @@
       <c r="N28" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O28" s="21" t="s">
+      <c r="O28" s="20" t="s">
         <v>64</v>
       </c>
       <c r="P28" s="22"/>
@@ -2316,7 +2308,7 @@
       <c r="N29" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O29" s="21" t="s">
+      <c r="O29" s="20" t="s">
         <v>65</v>
       </c>
       <c r="P29" s="22"/>
@@ -2337,7 +2329,7 @@
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
-      <c r="O30" s="21"/>
+      <c r="O30" s="20"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
@@ -2374,7 +2366,7 @@
         <v>68</v>
       </c>
       <c r="N31" s="15"/>
-      <c r="O31" s="21"/>
+      <c r="O31" s="20"/>
       <c r="P31" s="22"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
@@ -2393,7 +2385,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="21"/>
+      <c r="O32" s="20"/>
       <c r="P32" s="22"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
@@ -2423,7 +2415,7 @@
         <v>69</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="L33" s="15" t="s">
         <v>55</v>
@@ -2432,7 +2424,7 @@
         <v>68</v>
       </c>
       <c r="N33" s="16"/>
-      <c r="O33" s="21"/>
+      <c r="O33" s="20"/>
       <c r="P33" s="22"/>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
@@ -2477,7 +2469,7 @@
       <c r="N34" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="O34" s="21" t="s">
+      <c r="O34" s="20" t="s">
         <v>64</v>
       </c>
       <c r="P34" s="22"/>
@@ -2495,7 +2487,7 @@
       <c r="C35" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="20" t="s">
         <v>82</v>
       </c>
       <c r="E35" s="22"/>
@@ -2508,21 +2500,21 @@
       <c r="H35" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="I35" s="21" t="s">
+      <c r="I35" s="20" t="s">
         <v>84</v>
       </c>
       <c r="J35" s="22"/>
       <c r="K35" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="L35" s="21" t="s">
+      <c r="L35" s="20" t="s">
         <v>87</v>
       </c>
       <c r="M35" s="22"/>
-      <c r="N35" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="O35" s="23"/>
+      <c r="N35" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="O35" s="21"/>
       <c r="P35" s="22"/>
       <c r="Q35" s="15" t="s">
         <v>93</v>
@@ -2538,7 +2530,7 @@
       <c r="C36" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="20" t="s">
         <v>82</v>
       </c>
       <c r="E36" s="22"/>
@@ -2569,7 +2561,7 @@
       <c r="N36" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="O36" s="21" t="s">
+      <c r="O36" s="20" t="s">
         <v>81</v>
       </c>
       <c r="P36" s="22"/>
@@ -2587,7 +2579,7 @@
       <c r="C37" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="20" t="s">
         <v>92</v>
       </c>
       <c r="E37" s="22"/>
@@ -2615,10 +2607,10 @@
       <c r="M37" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="N37" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="O37" s="23"/>
+      <c r="N37" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="O37" s="21"/>
       <c r="P37" s="18"/>
       <c r="Q37" s="15" t="s">
         <v>82</v>
@@ -2636,6 +2628,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
     <mergeCell ref="N37:O37"/>
     <mergeCell ref="O27:P27"/>
     <mergeCell ref="O26:P26"/>
@@ -2652,38 +2676,6 @@
     <mergeCell ref="O31:P31"/>
     <mergeCell ref="O32:P32"/>
     <mergeCell ref="O33:P33"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2695,8 +2687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:P33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2723,22 +2715,22 @@
       <c r="B2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="24"/>
@@ -2767,7 +2759,7 @@
         <v>90</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="L3" s="11" t="s">
         <v>94</v>
@@ -2796,10 +2788,10 @@
         <v>100</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>103</v>
@@ -2814,7 +2806,7 @@
         <v>115</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>135</v>
+        <v>172</v>
       </c>
       <c r="L4" s="11" t="s">
         <v>117</v>
@@ -2826,7 +2818,7 @@
         <v>121</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="P4" s="11" t="s">
         <v>123</v>
@@ -2846,7 +2838,7 @@
         <v>101</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>104</v>
@@ -2861,7 +2853,7 @@
         <v>116</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>118</v>
@@ -2873,7 +2865,7 @@
         <v>122</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P5" s="11" t="s">
         <v>125</v>
@@ -2893,7 +2885,7 @@
         <v>101</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>105</v>
@@ -2908,7 +2900,7 @@
         <v>116</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>118</v>
@@ -2920,7 +2912,7 @@
         <v>122</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P6" s="11" t="s">
         <v>125</v>
@@ -2940,7 +2932,7 @@
         <v>101</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>106</v>
@@ -2955,7 +2947,7 @@
         <v>116</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L7" s="11" t="s">
         <v>118</v>
@@ -2967,7 +2959,7 @@
         <v>122</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P7" s="11" t="s">
         <v>124</v>
@@ -2987,7 +2979,7 @@
         <v>101</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>107</v>
@@ -3002,7 +2994,7 @@
         <v>116</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L8" s="11" t="s">
         <v>118</v>
@@ -3014,7 +3006,7 @@
         <v>122</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P8" s="11" t="s">
         <v>124</v>
@@ -3034,7 +3026,7 @@
         <v>101</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>108</v>
@@ -3049,7 +3041,7 @@
         <v>116</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L9" s="11" t="s">
         <v>118</v>
@@ -3061,7 +3053,7 @@
         <v>122</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P9" s="11" t="s">
         <v>124</v>
@@ -3081,7 +3073,7 @@
         <v>101</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>109</v>
@@ -3096,7 +3088,7 @@
         <v>116</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L10" s="11" t="s">
         <v>118</v>
@@ -3108,7 +3100,7 @@
         <v>122</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P10" s="11" t="s">
         <v>124</v>
@@ -3128,7 +3120,7 @@
         <v>101</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>110</v>
@@ -3143,7 +3135,7 @@
         <v>116</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L11" s="11" t="s">
         <v>118</v>
@@ -3155,7 +3147,7 @@
         <v>122</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P11" s="11" t="s">
         <v>124</v>
@@ -3192,7 +3184,7 @@
         <v>101</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>126</v>
@@ -3201,13 +3193,13 @@
         <v>112</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J13" s="14" t="s">
         <v>116</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L13" s="11" t="s">
         <v>118</v>
@@ -3219,7 +3211,7 @@
         <v>122</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P13" s="11" t="s">
         <v>125</v>
@@ -3239,7 +3231,7 @@
         <v>101</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>127</v>
@@ -3254,7 +3246,7 @@
         <v>116</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L14" s="11" t="s">
         <v>118</v>
@@ -3266,7 +3258,7 @@
         <v>122</v>
       </c>
       <c r="O14" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P14" s="11" t="s">
         <v>125</v>
@@ -3286,7 +3278,7 @@
         <v>101</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>128</v>
@@ -3301,7 +3293,7 @@
         <v>116</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L15" s="11" t="s">
         <v>118</v>
@@ -3313,7 +3305,7 @@
         <v>122</v>
       </c>
       <c r="O15" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>124</v>
@@ -3333,7 +3325,7 @@
         <v>101</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>129</v>
@@ -3348,7 +3340,7 @@
         <v>116</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L16" s="11" t="s">
         <v>118</v>
@@ -3360,7 +3352,7 @@
         <v>122</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>124</v>
@@ -3380,7 +3372,7 @@
         <v>101</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>130</v>
@@ -3395,7 +3387,7 @@
         <v>116</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L17" s="11" t="s">
         <v>118</v>
@@ -3407,7 +3399,7 @@
         <v>122</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P17" s="11" t="s">
         <v>124</v>
@@ -3427,7 +3419,7 @@
         <v>101</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>131</v>
@@ -3442,7 +3434,7 @@
         <v>116</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L18" s="11" t="s">
         <v>118</v>
@@ -3454,7 +3446,7 @@
         <v>122</v>
       </c>
       <c r="O18" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P18" s="11" t="s">
         <v>124</v>
@@ -3474,7 +3466,7 @@
         <v>101</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>132</v>
@@ -3489,7 +3481,7 @@
         <v>116</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L19" s="11" t="s">
         <v>118</v>
@@ -3501,7 +3493,7 @@
         <v>122</v>
       </c>
       <c r="O19" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P19" s="11" t="s">
         <v>124</v>
@@ -3518,10 +3510,10 @@
         <v>99</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>126</v>
@@ -3536,7 +3528,7 @@
         <v>116</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L20" s="11" t="s">
         <v>118</v>
@@ -3545,10 +3537,10 @@
         <v>120</v>
       </c>
       <c r="N20" s="11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="O20" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P20" s="11" t="s">
         <v>125</v>
@@ -3559,16 +3551,16 @@
         <v>46</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>99</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>126</v>
@@ -3583,7 +3575,7 @@
         <v>116</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L21" s="11" t="s">
         <v>118</v>
@@ -3595,10 +3587,10 @@
         <v>122</v>
       </c>
       <c r="O21" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P21" s="11" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -3626,13 +3618,13 @@
         <v>96</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>126</v>
@@ -3647,7 +3639,7 @@
         <v>116</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L23" s="11" t="s">
         <v>118</v>
@@ -3656,10 +3648,10 @@
         <v>120</v>
       </c>
       <c r="N23" s="11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="O23" s="11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="P23" s="11" t="s">
         <v>125</v>
@@ -3690,43 +3682,43 @@
         <v>97</v>
       </c>
       <c r="D25" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>156</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>126</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>133</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="L25" s="19" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="M25" s="19" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="N25" s="11" t="s">
         <v>122</v>
       </c>
       <c r="O25" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
@@ -3737,43 +3729,43 @@
         <v>97</v>
       </c>
       <c r="D26" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F26" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>156</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>126</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I26" s="17" t="s">
         <v>133</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="L26" s="19" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="M26" s="19" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="N26" s="11" t="s">
         <v>122</v>
       </c>
       <c r="O26" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
@@ -3784,43 +3776,43 @@
         <v>97</v>
       </c>
       <c r="D27" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F27" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>156</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>126</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>133</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="M27" s="19" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="N27" s="11" t="s">
         <v>122</v>
       </c>
       <c r="O27" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
@@ -3831,43 +3823,43 @@
         <v>97</v>
       </c>
       <c r="D28" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>156</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>126</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I28" s="17" t="s">
         <v>133</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="L28" s="19" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="M28" s="19" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="N28" s="11" t="s">
         <v>122</v>
       </c>
       <c r="O28" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
@@ -3901,13 +3893,13 @@
         <v>101</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I30" s="17" t="s">
         <v>133</v>
@@ -3916,7 +3908,7 @@
         <v>116</v>
       </c>
       <c r="K30" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L30" s="11" t="s">
         <v>118</v>
@@ -3928,7 +3920,7 @@
         <v>122</v>
       </c>
       <c r="O30" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P30" s="11" t="s">
         <v>125</v>
@@ -3956,22 +3948,22 @@
         <v>53</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>99</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>126</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I32" s="17" t="s">
         <v>133</v>
@@ -3980,7 +3972,7 @@
         <v>116</v>
       </c>
       <c r="K32" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L32" s="11" t="s">
         <v>118</v>
@@ -3992,10 +3984,10 @@
         <v>122</v>
       </c>
       <c r="O32" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P32" s="11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Lab2-1: implement IF & global params (#2)
* lab2-1: init commit

* Fix typo

* Update Datapath Control Sheet

* init vivado project `cpu`

* lab2-1: implement IF without test

* lab2-1: declare global control constant
</commit_message>
<xml_diff>
--- a/Datapath_Control_Sheet.xlsx
+++ b/Datapath_Control_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Project\iverilog\Exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B59DA3-2E5B-4EA5-9A6B-8B72782FA4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE605B31-6CC1-451B-B0F2-7FE2DB189768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据通路表(含控制信号)" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="178">
   <si>
     <t>所属单元</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -569,19 +569,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BrUnSel</t>
-  </si>
-  <si>
-    <t>BrUnSel_Non(3'b0)</t>
-  </si>
-  <si>
-    <t>BrUnSel_Non</t>
-  </si>
-  <si>
-    <t>BrUnSel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MemW_Non(1'b0)</t>
   </si>
   <si>
@@ -653,26 +640,6 @@
   </si>
   <si>
     <t>ImmSel_SB(3'b11)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BrUn_En(1'b1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BrUnSel_Beq(3'b1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BrUnSel_Bne(3'b10)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BrUnSel_Blt(3'b11)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BrUnSel_Bge(3'b100)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -746,6 +713,31 @@
     <t>A&lt;B?
 BrLT_T:BrLT_F</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BrSel</t>
+  </si>
+  <si>
+    <t>BrSel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BrSel_Non(3'b0)</t>
+  </si>
+  <si>
+    <t>BrSel_Non</t>
+  </si>
+  <si>
+    <t>BrSel_Beq(3'b1)</t>
+  </si>
+  <si>
+    <t>BrSel_Bne(3'b10)</t>
+  </si>
+  <si>
+    <t>BrSel_Blt(3'b11)</t>
+  </si>
+  <si>
+    <t>BrSel_Bge(3'b100)</t>
   </si>
 </sst>
 </file>
@@ -912,16 +904,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1243,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1273,30 +1265,30 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="21" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
       <c r="P2" s="22"/>
-      <c r="Q2" s="20" t="s">
+      <c r="Q2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="20"/>
+      <c r="R2" s="23"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1305,35 +1297,35 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
+      <c r="E3" s="23"/>
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21" t="s">
+      <c r="M3" s="23"/>
+      <c r="N3" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="O3" s="23"/>
+      <c r="O3" s="21"/>
       <c r="P3" s="22"/>
-      <c r="Q3" s="20" t="s">
+      <c r="Q3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="20"/>
+      <c r="R3" s="23"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1375,7 +1367,7 @@
       <c r="N4" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="20" t="s">
         <v>78</v>
       </c>
       <c r="P4" s="22"/>
@@ -1420,7 +1412,7 @@
         <v>65</v>
       </c>
       <c r="N5" s="15"/>
-      <c r="O5" s="21"/>
+      <c r="O5" s="20"/>
       <c r="P5" s="22"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="3"/>
@@ -1459,7 +1451,7 @@
         <v>65</v>
       </c>
       <c r="N6" s="15"/>
-      <c r="O6" s="21"/>
+      <c r="O6" s="20"/>
       <c r="P6" s="22"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="3"/>
@@ -1498,7 +1490,7 @@
         <v>64</v>
       </c>
       <c r="N7" s="15"/>
-      <c r="O7" s="21"/>
+      <c r="O7" s="20"/>
       <c r="P7" s="22"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="3"/>
@@ -1537,7 +1529,7 @@
         <v>64</v>
       </c>
       <c r="N8" s="15"/>
-      <c r="O8" s="21"/>
+      <c r="O8" s="20"/>
       <c r="P8" s="22"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="3"/>
@@ -1576,7 +1568,7 @@
         <v>64</v>
       </c>
       <c r="N9" s="15"/>
-      <c r="O9" s="21"/>
+      <c r="O9" s="20"/>
       <c r="P9" s="22"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="3"/>
@@ -1615,7 +1607,7 @@
         <v>64</v>
       </c>
       <c r="N10" s="15"/>
-      <c r="O10" s="21"/>
+      <c r="O10" s="20"/>
       <c r="P10" s="22"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="3"/>
@@ -1654,7 +1646,7 @@
         <v>64</v>
       </c>
       <c r="N11" s="15"/>
-      <c r="O11" s="21"/>
+      <c r="O11" s="20"/>
       <c r="P11" s="22"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="3"/>
@@ -1693,7 +1685,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="15"/>
-      <c r="O12" s="21"/>
+      <c r="O12" s="20"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="3"/>
@@ -1712,7 +1704,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="15"/>
-      <c r="O13" s="21"/>
+      <c r="O13" s="20"/>
       <c r="P13" s="22"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="3"/>
@@ -1751,7 +1743,7 @@
         <v>68</v>
       </c>
       <c r="N14" s="15"/>
-      <c r="O14" s="21"/>
+      <c r="O14" s="20"/>
       <c r="P14" s="22"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="3"/>
@@ -1790,7 +1782,7 @@
         <v>68</v>
       </c>
       <c r="N15" s="15"/>
-      <c r="O15" s="21"/>
+      <c r="O15" s="20"/>
       <c r="P15" s="22"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="3"/>
@@ -1829,7 +1821,7 @@
         <v>68</v>
       </c>
       <c r="N16" s="15"/>
-      <c r="O16" s="21"/>
+      <c r="O16" s="20"/>
       <c r="P16" s="22"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="3"/>
@@ -1868,7 +1860,7 @@
         <v>68</v>
       </c>
       <c r="N17" s="15"/>
-      <c r="O17" s="21"/>
+      <c r="O17" s="20"/>
       <c r="P17" s="22"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="3"/>
@@ -1907,7 +1899,7 @@
         <v>68</v>
       </c>
       <c r="N18" s="15"/>
-      <c r="O18" s="21"/>
+      <c r="O18" s="20"/>
       <c r="P18" s="22"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="3"/>
@@ -1946,7 +1938,7 @@
         <v>68</v>
       </c>
       <c r="N19" s="15"/>
-      <c r="O19" s="21"/>
+      <c r="O19" s="20"/>
       <c r="P19" s="22"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="3"/>
@@ -1985,7 +1977,7 @@
         <v>68</v>
       </c>
       <c r="N20" s="15"/>
-      <c r="O20" s="21"/>
+      <c r="O20" s="20"/>
       <c r="P20" s="22"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="3"/>
@@ -2024,7 +2016,7 @@
         <v>68</v>
       </c>
       <c r="N21" s="15"/>
-      <c r="O21" s="21"/>
+      <c r="O21" s="20"/>
       <c r="P21" s="22"/>
       <c r="Q21" s="6" t="s">
         <v>61</v>
@@ -2067,7 +2059,7 @@
         <v>68</v>
       </c>
       <c r="N22" s="15"/>
-      <c r="O22" s="21"/>
+      <c r="O22" s="20"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="3"/>
@@ -2086,7 +2078,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="15"/>
-      <c r="O23" s="21"/>
+      <c r="O23" s="20"/>
       <c r="P23" s="22"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="3"/>
@@ -2123,7 +2115,7 @@
         <v>68</v>
       </c>
       <c r="N24" s="15"/>
-      <c r="O24" s="21"/>
+      <c r="O24" s="20"/>
       <c r="P24" s="22"/>
       <c r="Q24" s="6" t="s">
         <v>61</v>
@@ -2146,7 +2138,7 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="15"/>
-      <c r="O25" s="21"/>
+      <c r="O25" s="20"/>
       <c r="P25" s="22"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="3"/>
@@ -2187,7 +2179,7 @@
       <c r="N26" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O26" s="21" t="s">
+      <c r="O26" s="20" t="s">
         <v>64</v>
       </c>
       <c r="P26" s="22"/>
@@ -2230,7 +2222,7 @@
       <c r="N27" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O27" s="21" t="s">
+      <c r="O27" s="20" t="s">
         <v>64</v>
       </c>
       <c r="P27" s="22"/>
@@ -2273,7 +2265,7 @@
       <c r="N28" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O28" s="21" t="s">
+      <c r="O28" s="20" t="s">
         <v>64</v>
       </c>
       <c r="P28" s="22"/>
@@ -2316,7 +2308,7 @@
       <c r="N29" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O29" s="21" t="s">
+      <c r="O29" s="20" t="s">
         <v>65</v>
       </c>
       <c r="P29" s="22"/>
@@ -2337,7 +2329,7 @@
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
-      <c r="O30" s="21"/>
+      <c r="O30" s="20"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
@@ -2374,7 +2366,7 @@
         <v>68</v>
       </c>
       <c r="N31" s="15"/>
-      <c r="O31" s="21"/>
+      <c r="O31" s="20"/>
       <c r="P31" s="22"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
@@ -2393,7 +2385,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="21"/>
+      <c r="O32" s="20"/>
       <c r="P32" s="22"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
@@ -2423,7 +2415,7 @@
         <v>69</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="L33" s="15" t="s">
         <v>55</v>
@@ -2432,7 +2424,7 @@
         <v>68</v>
       </c>
       <c r="N33" s="16"/>
-      <c r="O33" s="21"/>
+      <c r="O33" s="20"/>
       <c r="P33" s="22"/>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
@@ -2477,7 +2469,7 @@
       <c r="N34" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="O34" s="21" t="s">
+      <c r="O34" s="20" t="s">
         <v>64</v>
       </c>
       <c r="P34" s="22"/>
@@ -2495,7 +2487,7 @@
       <c r="C35" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="20" t="s">
         <v>82</v>
       </c>
       <c r="E35" s="22"/>
@@ -2508,21 +2500,21 @@
       <c r="H35" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="I35" s="21" t="s">
+      <c r="I35" s="20" t="s">
         <v>84</v>
       </c>
       <c r="J35" s="22"/>
       <c r="K35" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="L35" s="21" t="s">
+      <c r="L35" s="20" t="s">
         <v>87</v>
       </c>
       <c r="M35" s="22"/>
-      <c r="N35" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="O35" s="23"/>
+      <c r="N35" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="O35" s="21"/>
       <c r="P35" s="22"/>
       <c r="Q35" s="15" t="s">
         <v>93</v>
@@ -2538,7 +2530,7 @@
       <c r="C36" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="20" t="s">
         <v>82</v>
       </c>
       <c r="E36" s="22"/>
@@ -2569,7 +2561,7 @@
       <c r="N36" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="O36" s="21" t="s">
+      <c r="O36" s="20" t="s">
         <v>81</v>
       </c>
       <c r="P36" s="22"/>
@@ -2587,7 +2579,7 @@
       <c r="C37" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="20" t="s">
         <v>92</v>
       </c>
       <c r="E37" s="22"/>
@@ -2615,10 +2607,10 @@
       <c r="M37" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="N37" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="O37" s="23"/>
+      <c r="N37" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="O37" s="21"/>
       <c r="P37" s="18"/>
       <c r="Q37" s="15" t="s">
         <v>82</v>
@@ -2636,6 +2628,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
     <mergeCell ref="N37:O37"/>
     <mergeCell ref="O27:P27"/>
     <mergeCell ref="O26:P26"/>
@@ -2652,38 +2676,6 @@
     <mergeCell ref="O31:P31"/>
     <mergeCell ref="O32:P32"/>
     <mergeCell ref="O33:P33"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2695,8 +2687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:P33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2723,22 +2715,22 @@
       <c r="B2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="24"/>
@@ -2767,7 +2759,7 @@
         <v>90</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="L3" s="11" t="s">
         <v>94</v>
@@ -2796,10 +2788,10 @@
         <v>100</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>103</v>
@@ -2814,7 +2806,7 @@
         <v>115</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>135</v>
+        <v>172</v>
       </c>
       <c r="L4" s="11" t="s">
         <v>117</v>
@@ -2826,7 +2818,7 @@
         <v>121</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="P4" s="11" t="s">
         <v>123</v>
@@ -2846,7 +2838,7 @@
         <v>101</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>104</v>
@@ -2861,7 +2853,7 @@
         <v>116</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>118</v>
@@ -2873,7 +2865,7 @@
         <v>122</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P5" s="11" t="s">
         <v>125</v>
@@ -2893,7 +2885,7 @@
         <v>101</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>105</v>
@@ -2908,7 +2900,7 @@
         <v>116</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>118</v>
@@ -2920,7 +2912,7 @@
         <v>122</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P6" s="11" t="s">
         <v>125</v>
@@ -2940,7 +2932,7 @@
         <v>101</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>106</v>
@@ -2955,7 +2947,7 @@
         <v>116</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L7" s="11" t="s">
         <v>118</v>
@@ -2967,7 +2959,7 @@
         <v>122</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P7" s="11" t="s">
         <v>124</v>
@@ -2987,7 +2979,7 @@
         <v>101</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>107</v>
@@ -3002,7 +2994,7 @@
         <v>116</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L8" s="11" t="s">
         <v>118</v>
@@ -3014,7 +3006,7 @@
         <v>122</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P8" s="11" t="s">
         <v>124</v>
@@ -3034,7 +3026,7 @@
         <v>101</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>108</v>
@@ -3049,7 +3041,7 @@
         <v>116</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L9" s="11" t="s">
         <v>118</v>
@@ -3061,7 +3053,7 @@
         <v>122</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P9" s="11" t="s">
         <v>124</v>
@@ -3081,7 +3073,7 @@
         <v>101</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>109</v>
@@ -3096,7 +3088,7 @@
         <v>116</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L10" s="11" t="s">
         <v>118</v>
@@ -3108,7 +3100,7 @@
         <v>122</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P10" s="11" t="s">
         <v>124</v>
@@ -3128,7 +3120,7 @@
         <v>101</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>110</v>
@@ -3143,7 +3135,7 @@
         <v>116</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L11" s="11" t="s">
         <v>118</v>
@@ -3155,7 +3147,7 @@
         <v>122</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P11" s="11" t="s">
         <v>124</v>
@@ -3192,7 +3184,7 @@
         <v>101</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>126</v>
@@ -3201,13 +3193,13 @@
         <v>112</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J13" s="14" t="s">
         <v>116</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L13" s="11" t="s">
         <v>118</v>
@@ -3219,7 +3211,7 @@
         <v>122</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P13" s="11" t="s">
         <v>125</v>
@@ -3239,7 +3231,7 @@
         <v>101</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>127</v>
@@ -3254,7 +3246,7 @@
         <v>116</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L14" s="11" t="s">
         <v>118</v>
@@ -3266,7 +3258,7 @@
         <v>122</v>
       </c>
       <c r="O14" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P14" s="11" t="s">
         <v>125</v>
@@ -3286,7 +3278,7 @@
         <v>101</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>128</v>
@@ -3301,7 +3293,7 @@
         <v>116</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L15" s="11" t="s">
         <v>118</v>
@@ -3313,7 +3305,7 @@
         <v>122</v>
       </c>
       <c r="O15" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>124</v>
@@ -3333,7 +3325,7 @@
         <v>101</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>129</v>
@@ -3348,7 +3340,7 @@
         <v>116</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L16" s="11" t="s">
         <v>118</v>
@@ -3360,7 +3352,7 @@
         <v>122</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>124</v>
@@ -3380,7 +3372,7 @@
         <v>101</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>130</v>
@@ -3395,7 +3387,7 @@
         <v>116</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L17" s="11" t="s">
         <v>118</v>
@@ -3407,7 +3399,7 @@
         <v>122</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P17" s="11" t="s">
         <v>124</v>
@@ -3427,7 +3419,7 @@
         <v>101</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>131</v>
@@ -3442,7 +3434,7 @@
         <v>116</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L18" s="11" t="s">
         <v>118</v>
@@ -3454,7 +3446,7 @@
         <v>122</v>
       </c>
       <c r="O18" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P18" s="11" t="s">
         <v>124</v>
@@ -3474,7 +3466,7 @@
         <v>101</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>132</v>
@@ -3489,7 +3481,7 @@
         <v>116</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L19" s="11" t="s">
         <v>118</v>
@@ -3501,7 +3493,7 @@
         <v>122</v>
       </c>
       <c r="O19" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P19" s="11" t="s">
         <v>124</v>
@@ -3518,10 +3510,10 @@
         <v>99</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>126</v>
@@ -3536,7 +3528,7 @@
         <v>116</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L20" s="11" t="s">
         <v>118</v>
@@ -3545,10 +3537,10 @@
         <v>120</v>
       </c>
       <c r="N20" s="11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="O20" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P20" s="11" t="s">
         <v>125</v>
@@ -3559,16 +3551,16 @@
         <v>46</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>99</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>126</v>
@@ -3583,7 +3575,7 @@
         <v>116</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L21" s="11" t="s">
         <v>118</v>
@@ -3595,10 +3587,10 @@
         <v>122</v>
       </c>
       <c r="O21" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P21" s="11" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -3626,13 +3618,13 @@
         <v>96</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>126</v>
@@ -3647,7 +3639,7 @@
         <v>116</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L23" s="11" t="s">
         <v>118</v>
@@ -3656,10 +3648,10 @@
         <v>120</v>
       </c>
       <c r="N23" s="11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="O23" s="11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="P23" s="11" t="s">
         <v>125</v>
@@ -3690,43 +3682,43 @@
         <v>97</v>
       </c>
       <c r="D25" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>156</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>126</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>133</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="L25" s="19" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="M25" s="19" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="N25" s="11" t="s">
         <v>122</v>
       </c>
       <c r="O25" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
@@ -3737,43 +3729,43 @@
         <v>97</v>
       </c>
       <c r="D26" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F26" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>156</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>126</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I26" s="17" t="s">
         <v>133</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="L26" s="19" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="M26" s="19" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="N26" s="11" t="s">
         <v>122</v>
       </c>
       <c r="O26" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
@@ -3784,43 +3776,43 @@
         <v>97</v>
       </c>
       <c r="D27" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F27" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>156</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>126</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>133</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="M27" s="19" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="N27" s="11" t="s">
         <v>122</v>
       </c>
       <c r="O27" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
@@ -3831,43 +3823,43 @@
         <v>97</v>
       </c>
       <c r="D28" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>156</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>126</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I28" s="17" t="s">
         <v>133</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="L28" s="19" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="M28" s="19" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="N28" s="11" t="s">
         <v>122</v>
       </c>
       <c r="O28" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
@@ -3901,13 +3893,13 @@
         <v>101</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I30" s="17" t="s">
         <v>133</v>
@@ -3916,7 +3908,7 @@
         <v>116</v>
       </c>
       <c r="K30" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L30" s="11" t="s">
         <v>118</v>
@@ -3928,7 +3920,7 @@
         <v>122</v>
       </c>
       <c r="O30" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P30" s="11" t="s">
         <v>125</v>
@@ -3956,22 +3948,22 @@
         <v>53</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>99</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>126</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I32" s="17" t="s">
         <v>133</v>
@@ -3980,7 +3972,7 @@
         <v>116</v>
       </c>
       <c r="K32" s="11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="L32" s="11" t="s">
         <v>118</v>
@@ -3992,10 +3984,10 @@
         <v>122</v>
       </c>
       <c r="O32" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P32" s="11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update xlsx & Update all `.v` file, aka. format the code
</commit_message>
<xml_diff>
--- a/Datapath_Control_Sheet.xlsx
+++ b/Datapath_Control_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Project\iverilog\Exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE605B31-6CC1-451B-B0F2-7FE2DB189768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D69C78-D213-43B2-9552-9696F54AD232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据通路表(含控制信号)" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="180">
   <si>
     <t>所属单元</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -738,6 +738,14 @@
   </si>
   <si>
     <t>BrSel_Bge(3'b100)</t>
+  </si>
+  <si>
+    <t>ImmSel_IS(3'b110)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ImmSel_IS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -904,16 +912,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1235,99 +1243,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="9.375" customWidth="1"/>
-    <col min="4" max="4" width="9.625" customWidth="1"/>
-    <col min="5" max="5" width="8.75" customWidth="1"/>
-    <col min="6" max="6" width="8.875" customWidth="1"/>
-    <col min="7" max="7" width="14.125" customWidth="1"/>
+    <col min="1" max="1" width="3.4609375" customWidth="1"/>
+    <col min="2" max="2" width="10.4609375" customWidth="1"/>
+    <col min="3" max="3" width="9.3828125" customWidth="1"/>
+    <col min="4" max="4" width="9.61328125" customWidth="1"/>
+    <col min="5" max="5" width="8.765625" customWidth="1"/>
+    <col min="6" max="6" width="8.84375" customWidth="1"/>
+    <col min="7" max="7" width="14.15234375" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="16.875" customWidth="1"/>
-    <col min="10" max="10" width="15.125" customWidth="1"/>
-    <col min="11" max="11" width="33.5" customWidth="1"/>
-    <col min="12" max="12" width="12.5" customWidth="1"/>
-    <col min="13" max="13" width="9.125" customWidth="1"/>
-    <col min="14" max="14" width="7.625" customWidth="1"/>
-    <col min="15" max="15" width="9.25" customWidth="1"/>
-    <col min="16" max="16" width="0.25" customWidth="1"/>
-    <col min="17" max="17" width="8.625" customWidth="1"/>
-    <col min="18" max="18" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="16.84375" customWidth="1"/>
+    <col min="10" max="10" width="15.15234375" customWidth="1"/>
+    <col min="11" max="11" width="33.4609375" customWidth="1"/>
+    <col min="12" max="12" width="12.4609375" customWidth="1"/>
+    <col min="13" max="13" width="9.15234375" customWidth="1"/>
+    <col min="14" max="14" width="7.61328125" customWidth="1"/>
+    <col min="15" max="15" width="9.23046875" customWidth="1"/>
+    <col min="16" max="16" width="0.23046875" customWidth="1"/>
+    <col min="17" max="17" width="8.61328125" customWidth="1"/>
+    <col min="18" max="18" width="9.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="20" t="s">
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
       <c r="P2" s="22"/>
-      <c r="Q2" s="23" t="s">
+      <c r="Q2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="23"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R2" s="20"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="23"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
       <c r="K3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="20" t="s">
+      <c r="M3" s="20"/>
+      <c r="N3" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="O3" s="21"/>
+      <c r="O3" s="23"/>
       <c r="P3" s="22"/>
-      <c r="Q3" s="23" t="s">
+      <c r="Q3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="23"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R3" s="20"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1367,7 +1375,7 @@
       <c r="N4" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="O4" s="21" t="s">
         <v>78</v>
       </c>
       <c r="P4" s="22"/>
@@ -1378,7 +1386,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
         <v>30</v>
       </c>
@@ -1412,12 +1420,12 @@
         <v>65</v>
       </c>
       <c r="N5" s="15"/>
-      <c r="O5" s="20"/>
+      <c r="O5" s="21"/>
       <c r="P5" s="22"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>31</v>
       </c>
@@ -1451,12 +1459,12 @@
         <v>65</v>
       </c>
       <c r="N6" s="15"/>
-      <c r="O6" s="20"/>
+      <c r="O6" s="21"/>
       <c r="P6" s="22"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>32</v>
       </c>
@@ -1490,12 +1498,12 @@
         <v>64</v>
       </c>
       <c r="N7" s="15"/>
-      <c r="O7" s="20"/>
+      <c r="O7" s="21"/>
       <c r="P7" s="22"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>33</v>
       </c>
@@ -1529,12 +1537,12 @@
         <v>64</v>
       </c>
       <c r="N8" s="15"/>
-      <c r="O8" s="20"/>
+      <c r="O8" s="21"/>
       <c r="P8" s="22"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
         <v>34</v>
       </c>
@@ -1568,12 +1576,12 @@
         <v>64</v>
       </c>
       <c r="N9" s="15"/>
-      <c r="O9" s="20"/>
+      <c r="O9" s="21"/>
       <c r="P9" s="22"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
         <v>35</v>
       </c>
@@ -1607,12 +1615,12 @@
         <v>64</v>
       </c>
       <c r="N10" s="15"/>
-      <c r="O10" s="20"/>
+      <c r="O10" s="21"/>
       <c r="P10" s="22"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
         <v>36</v>
       </c>
@@ -1646,12 +1654,12 @@
         <v>64</v>
       </c>
       <c r="N11" s="15"/>
-      <c r="O11" s="20"/>
+      <c r="O11" s="21"/>
       <c r="P11" s="22"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
         <v>37</v>
       </c>
@@ -1685,12 +1693,12 @@
         <v>64</v>
       </c>
       <c r="N12" s="15"/>
-      <c r="O12" s="20"/>
+      <c r="O12" s="21"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -1704,12 +1712,12 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="15"/>
-      <c r="O13" s="20"/>
+      <c r="O13" s="21"/>
       <c r="P13" s="22"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
         <v>38</v>
       </c>
@@ -1743,12 +1751,12 @@
         <v>68</v>
       </c>
       <c r="N14" s="15"/>
-      <c r="O14" s="20"/>
+      <c r="O14" s="21"/>
       <c r="P14" s="22"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="3"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
         <v>39</v>
       </c>
@@ -1782,12 +1790,12 @@
         <v>68</v>
       </c>
       <c r="N15" s="15"/>
-      <c r="O15" s="20"/>
+      <c r="O15" s="21"/>
       <c r="P15" s="22"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B16" s="6" t="s">
         <v>40</v>
       </c>
@@ -1821,12 +1829,12 @@
         <v>68</v>
       </c>
       <c r="N16" s="15"/>
-      <c r="O16" s="20"/>
+      <c r="O16" s="21"/>
       <c r="P16" s="22"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
         <v>41</v>
       </c>
@@ -1860,12 +1868,12 @@
         <v>68</v>
       </c>
       <c r="N17" s="15"/>
-      <c r="O17" s="20"/>
+      <c r="O17" s="21"/>
       <c r="P17" s="22"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="3"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1890,7 +1898,7 @@
         <v>61</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="L18" s="15" t="s">
         <v>62</v>
@@ -1899,12 +1907,12 @@
         <v>68</v>
       </c>
       <c r="N18" s="15"/>
-      <c r="O18" s="20"/>
+      <c r="O18" s="21"/>
       <c r="P18" s="22"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="3"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
         <v>43</v>
       </c>
@@ -1929,7 +1937,7 @@
         <v>61</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="L19" s="15" t="s">
         <v>62</v>
@@ -1938,12 +1946,12 @@
         <v>68</v>
       </c>
       <c r="N19" s="15"/>
-      <c r="O19" s="20"/>
+      <c r="O19" s="21"/>
       <c r="P19" s="22"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="3"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B20" s="6" t="s">
         <v>44</v>
       </c>
@@ -1968,7 +1976,7 @@
         <v>61</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="L20" s="15" t="s">
         <v>62</v>
@@ -1977,12 +1985,12 @@
         <v>68</v>
       </c>
       <c r="N20" s="15"/>
-      <c r="O20" s="20"/>
+      <c r="O20" s="21"/>
       <c r="P20" s="22"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="3"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
         <v>45</v>
       </c>
@@ -2016,14 +2024,14 @@
         <v>68</v>
       </c>
       <c r="N21" s="15"/>
-      <c r="O21" s="20"/>
+      <c r="O21" s="21"/>
       <c r="P21" s="22"/>
       <c r="Q21" s="6" t="s">
         <v>61</v>
       </c>
       <c r="R21" s="3"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
         <v>46</v>
       </c>
@@ -2059,12 +2067,12 @@
         <v>68</v>
       </c>
       <c r="N22" s="15"/>
-      <c r="O22" s="20"/>
+      <c r="O22" s="21"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="3"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B23" s="6"/>
       <c r="C23" s="15"/>
       <c r="D23" s="6"/>
@@ -2078,12 +2086,12 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="15"/>
-      <c r="O23" s="20"/>
+      <c r="O23" s="21"/>
       <c r="P23" s="22"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
         <v>47</v>
       </c>
@@ -2115,7 +2123,7 @@
         <v>68</v>
       </c>
       <c r="N24" s="15"/>
-      <c r="O24" s="20"/>
+      <c r="O24" s="21"/>
       <c r="P24" s="22"/>
       <c r="Q24" s="6" t="s">
         <v>61</v>
@@ -2124,7 +2132,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B25" s="6"/>
       <c r="C25" s="15"/>
       <c r="D25" s="6"/>
@@ -2138,12 +2146,12 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="15"/>
-      <c r="O25" s="20"/>
+      <c r="O25" s="21"/>
       <c r="P25" s="22"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="3"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
         <v>48</v>
       </c>
@@ -2179,14 +2187,14 @@
       <c r="N26" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O26" s="20" t="s">
+      <c r="O26" s="21" t="s">
         <v>64</v>
       </c>
       <c r="P26" s="22"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="3"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
         <v>49</v>
       </c>
@@ -2222,14 +2230,14 @@
       <c r="N27" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O27" s="20" t="s">
+      <c r="O27" s="21" t="s">
         <v>64</v>
       </c>
       <c r="P27" s="22"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="3"/>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B28" s="15" t="s">
         <v>50</v>
       </c>
@@ -2265,14 +2273,14 @@
       <c r="N28" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O28" s="20" t="s">
+      <c r="O28" s="21" t="s">
         <v>64</v>
       </c>
       <c r="P28" s="22"/>
       <c r="Q28" s="15"/>
       <c r="R28" s="3"/>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B29" s="15" t="s">
         <v>51</v>
       </c>
@@ -2308,14 +2316,14 @@
       <c r="N29" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O29" s="20" t="s">
+      <c r="O29" s="21" t="s">
         <v>65</v>
       </c>
       <c r="P29" s="22"/>
       <c r="Q29" s="15"/>
       <c r="R29" s="3"/>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -2329,12 +2337,12 @@
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
-      <c r="O30" s="20"/>
+      <c r="O30" s="21"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
     </row>
-    <row r="31" spans="2:18" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" ht="31" x14ac:dyDescent="0.35">
       <c r="B31" s="15" t="s">
         <v>52</v>
       </c>
@@ -2366,12 +2374,12 @@
         <v>68</v>
       </c>
       <c r="N31" s="15"/>
-      <c r="O31" s="20"/>
+      <c r="O31" s="21"/>
       <c r="P31" s="22"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B32" s="15"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2385,12 +2393,12 @@
       <c r="L32" s="2"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="20"/>
+      <c r="O32" s="21"/>
       <c r="P32" s="22"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>53</v>
       </c>
@@ -2424,12 +2432,12 @@
         <v>68</v>
       </c>
       <c r="N33" s="16"/>
-      <c r="O33" s="20"/>
+      <c r="O33" s="21"/>
       <c r="P33" s="22"/>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
     </row>
-    <row r="34" spans="2:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
         <v>22</v>
       </c>
@@ -2469,7 +2477,7 @@
       <c r="N34" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="O34" s="20" t="s">
+      <c r="O34" s="21" t="s">
         <v>64</v>
       </c>
       <c r="P34" s="22"/>
@@ -2480,14 +2488,14 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B35" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="D35" s="21" t="s">
         <v>82</v>
       </c>
       <c r="E35" s="22"/>
@@ -2500,21 +2508,21 @@
       <c r="H35" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="I35" s="20" t="s">
+      <c r="I35" s="21" t="s">
         <v>84</v>
       </c>
       <c r="J35" s="22"/>
       <c r="K35" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="L35" s="20" t="s">
+      <c r="L35" s="21" t="s">
         <v>87</v>
       </c>
       <c r="M35" s="22"/>
-      <c r="N35" s="20" t="s">
+      <c r="N35" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="O35" s="21"/>
+      <c r="O35" s="23"/>
       <c r="P35" s="22"/>
       <c r="Q35" s="15" t="s">
         <v>93</v>
@@ -2523,14 +2531,14 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B36" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D36" s="21" t="s">
         <v>82</v>
       </c>
       <c r="E36" s="22"/>
@@ -2561,7 +2569,7 @@
       <c r="N36" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="O36" s="20" t="s">
+      <c r="O36" s="21" t="s">
         <v>81</v>
       </c>
       <c r="P36" s="22"/>
@@ -2572,14 +2580,14 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B37" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="21" t="s">
         <v>92</v>
       </c>
       <c r="E37" s="22"/>
@@ -2607,10 +2615,10 @@
       <c r="M37" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="N37" s="20" t="s">
+      <c r="N37" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="O37" s="21"/>
+      <c r="O37" s="23"/>
       <c r="P37" s="18"/>
       <c r="Q37" s="15" t="s">
         <v>82</v>
@@ -2619,47 +2627,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.35">
       <c r="C38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B40" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
     <mergeCell ref="N37:O37"/>
     <mergeCell ref="O27:P27"/>
     <mergeCell ref="O26:P26"/>
@@ -2676,6 +2652,38 @@
     <mergeCell ref="O31:P31"/>
     <mergeCell ref="O32:P32"/>
     <mergeCell ref="O33:P33"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2688,51 +2696,51 @@
   <dimension ref="B2:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.75" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="19.875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="9" customWidth="1"/>
-    <col min="6" max="6" width="17.375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="19.5" style="9" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="9" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="15.25" style="9" customWidth="1"/>
-    <col min="11" max="11" width="20.75" style="9" customWidth="1"/>
-    <col min="12" max="12" width="18.75" style="9" customWidth="1"/>
-    <col min="13" max="13" width="15.25" style="9" customWidth="1"/>
-    <col min="14" max="14" width="15.875" style="9" customWidth="1"/>
-    <col min="15" max="15" width="16.625" style="9" customWidth="1"/>
-    <col min="16" max="16" width="26.125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="3.765625" customWidth="1"/>
+    <col min="2" max="2" width="7.15234375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="18.15234375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="19.84375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="18.4609375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.3828125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="19.4609375" style="9" customWidth="1"/>
+    <col min="8" max="8" width="13.4609375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="10.84375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="15.23046875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="20.765625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="18.765625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="15.23046875" style="9" customWidth="1"/>
+    <col min="14" max="14" width="15.84375" style="9" customWidth="1"/>
+    <col min="15" max="15" width="16.61328125" style="9" customWidth="1"/>
+    <col min="16" max="16" width="26.15234375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B3" s="24"/>
       <c r="C3" s="10" t="s">
         <v>83</v>
@@ -2777,7 +2785,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" s="15" t="s">
         <v>30</v>
       </c>
@@ -2824,7 +2832,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" s="15" t="s">
         <v>31</v>
       </c>
@@ -2871,7 +2879,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
         <v>32</v>
       </c>
@@ -2918,7 +2926,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
         <v>33</v>
       </c>
@@ -2965,7 +2973,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
         <v>34</v>
       </c>
@@ -3012,7 +3020,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9" s="15" t="s">
         <v>35</v>
       </c>
@@ -3059,7 +3067,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B10" s="15" t="s">
         <v>36</v>
       </c>
@@ -3106,7 +3114,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B11" s="15" t="s">
         <v>37</v>
       </c>
@@ -3153,7 +3161,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B12" s="15"/>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
@@ -3170,7 +3178,7 @@
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B13" s="15" t="s">
         <v>38</v>
       </c>
@@ -3217,7 +3225,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B14" s="15" t="s">
         <v>39</v>
       </c>
@@ -3264,7 +3272,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B15" s="15" t="s">
         <v>40</v>
       </c>
@@ -3311,7 +3319,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B16" s="15" t="s">
         <v>41</v>
       </c>
@@ -3358,7 +3366,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B17" s="15" t="s">
         <v>42</v>
       </c>
@@ -3372,7 +3380,7 @@
         <v>101</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>130</v>
@@ -3405,7 +3413,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B18" s="15" t="s">
         <v>43</v>
       </c>
@@ -3419,7 +3427,7 @@
         <v>101</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>131</v>
@@ -3452,7 +3460,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B19" s="15" t="s">
         <v>44</v>
       </c>
@@ -3466,7 +3474,7 @@
         <v>101</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>132</v>
@@ -3499,7 +3507,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B20" s="15" t="s">
         <v>45</v>
       </c>
@@ -3546,7 +3554,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B21" s="15" t="s">
         <v>46</v>
       </c>
@@ -3593,7 +3601,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B22" s="15"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -3610,7 +3618,7 @@
       <c r="O22" s="15"/>
       <c r="P22" s="6"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B23" s="15" t="s">
         <v>47</v>
       </c>
@@ -3657,7 +3665,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B24" s="15"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -3674,7 +3682,7 @@
       <c r="O24" s="15"/>
       <c r="P24" s="6"/>
     </row>
-    <row r="25" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" ht="31" x14ac:dyDescent="0.35">
       <c r="B25" s="15" t="s">
         <v>48</v>
       </c>
@@ -3721,7 +3729,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" ht="31" x14ac:dyDescent="0.35">
       <c r="B26" s="15" t="s">
         <v>49</v>
       </c>
@@ -3768,7 +3776,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" ht="31" x14ac:dyDescent="0.35">
       <c r="B27" s="15" t="s">
         <v>50</v>
       </c>
@@ -3815,7 +3823,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" ht="31" x14ac:dyDescent="0.35">
       <c r="B28" s="15" t="s">
         <v>51</v>
       </c>
@@ -3862,7 +3870,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B29" s="15"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -3879,7 +3887,7 @@
       <c r="O29" s="15"/>
       <c r="P29" s="6"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B30" s="15" t="s">
         <v>52</v>
       </c>
@@ -3926,7 +3934,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -3943,7 +3951,7 @@
       <c r="O31" s="15"/>
       <c r="P31" s="15"/>
     </row>
-    <row r="32" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="15" t="s">
         <v>53</v>
       </c>
@@ -3990,7 +3998,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>

</xml_diff>

<commit_message>
lab2-1-test: implement `comp.v` & `exe_top.v` without test
</commit_message>
<xml_diff>
--- a/Datapath_Control_Sheet.xlsx
+++ b/Datapath_Control_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Project\iverilog\Exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D69C78-D213-43B2-9552-9696F54AD232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C2EDC6-810B-4A55-AB18-06DD7ECD777B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据通路表(含控制信号)" sheetId="1" r:id="rId1"/>
@@ -912,16 +912,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1243,99 +1243,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.4609375" customWidth="1"/>
-    <col min="2" max="2" width="10.4609375" customWidth="1"/>
-    <col min="3" max="3" width="9.3828125" customWidth="1"/>
-    <col min="4" max="4" width="9.61328125" customWidth="1"/>
-    <col min="5" max="5" width="8.765625" customWidth="1"/>
-    <col min="6" max="6" width="8.84375" customWidth="1"/>
-    <col min="7" max="7" width="14.15234375" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="9.375" customWidth="1"/>
+    <col min="4" max="4" width="9.625" customWidth="1"/>
+    <col min="5" max="5" width="8.75" customWidth="1"/>
+    <col min="6" max="6" width="8.875" customWidth="1"/>
+    <col min="7" max="7" width="14.125" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="16.84375" customWidth="1"/>
-    <col min="10" max="10" width="15.15234375" customWidth="1"/>
-    <col min="11" max="11" width="33.4609375" customWidth="1"/>
-    <col min="12" max="12" width="12.4609375" customWidth="1"/>
-    <col min="13" max="13" width="9.15234375" customWidth="1"/>
-    <col min="14" max="14" width="7.61328125" customWidth="1"/>
-    <col min="15" max="15" width="9.23046875" customWidth="1"/>
-    <col min="16" max="16" width="0.23046875" customWidth="1"/>
-    <col min="17" max="17" width="8.61328125" customWidth="1"/>
-    <col min="18" max="18" width="9.4609375" customWidth="1"/>
+    <col min="9" max="9" width="16.875" customWidth="1"/>
+    <col min="10" max="10" width="15.125" customWidth="1"/>
+    <col min="11" max="11" width="33.5" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
+    <col min="13" max="13" width="9.125" customWidth="1"/>
+    <col min="14" max="14" width="7.625" customWidth="1"/>
+    <col min="15" max="15" width="9.25" customWidth="1"/>
+    <col min="16" max="16" width="0.25" customWidth="1"/>
+    <col min="17" max="17" width="8.625" customWidth="1"/>
+    <col min="18" max="18" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="21" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
       <c r="P2" s="22"/>
-      <c r="Q2" s="20" t="s">
+      <c r="Q2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="20"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="R2" s="23"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
+      <c r="E3" s="23"/>
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21" t="s">
+      <c r="M3" s="23"/>
+      <c r="N3" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="O3" s="23"/>
+      <c r="O3" s="21"/>
       <c r="P3" s="22"/>
-      <c r="Q3" s="20" t="s">
+      <c r="Q3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="20"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="R3" s="23"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1375,7 +1375,7 @@
       <c r="N4" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="20" t="s">
         <v>78</v>
       </c>
       <c r="P4" s="22"/>
@@ -1386,7 +1386,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>30</v>
       </c>
@@ -1420,12 +1420,12 @@
         <v>65</v>
       </c>
       <c r="N5" s="15"/>
-      <c r="O5" s="21"/>
+      <c r="O5" s="20"/>
       <c r="P5" s="22"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>31</v>
       </c>
@@ -1459,12 +1459,12 @@
         <v>65</v>
       </c>
       <c r="N6" s="15"/>
-      <c r="O6" s="21"/>
+      <c r="O6" s="20"/>
       <c r="P6" s="22"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>32</v>
       </c>
@@ -1498,12 +1498,12 @@
         <v>64</v>
       </c>
       <c r="N7" s="15"/>
-      <c r="O7" s="21"/>
+      <c r="O7" s="20"/>
       <c r="P7" s="22"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>33</v>
       </c>
@@ -1537,12 +1537,12 @@
         <v>64</v>
       </c>
       <c r="N8" s="15"/>
-      <c r="O8" s="21"/>
+      <c r="O8" s="20"/>
       <c r="P8" s="22"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>34</v>
       </c>
@@ -1576,12 +1576,12 @@
         <v>64</v>
       </c>
       <c r="N9" s="15"/>
-      <c r="O9" s="21"/>
+      <c r="O9" s="20"/>
       <c r="P9" s="22"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>35</v>
       </c>
@@ -1615,12 +1615,12 @@
         <v>64</v>
       </c>
       <c r="N10" s="15"/>
-      <c r="O10" s="21"/>
+      <c r="O10" s="20"/>
       <c r="P10" s="22"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>36</v>
       </c>
@@ -1654,12 +1654,12 @@
         <v>64</v>
       </c>
       <c r="N11" s="15"/>
-      <c r="O11" s="21"/>
+      <c r="O11" s="20"/>
       <c r="P11" s="22"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>37</v>
       </c>
@@ -1693,12 +1693,12 @@
         <v>64</v>
       </c>
       <c r="N12" s="15"/>
-      <c r="O12" s="21"/>
+      <c r="O12" s="20"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -1712,12 +1712,12 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="15"/>
-      <c r="O13" s="21"/>
+      <c r="O13" s="20"/>
       <c r="P13" s="22"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>38</v>
       </c>
@@ -1751,12 +1751,12 @@
         <v>68</v>
       </c>
       <c r="N14" s="15"/>
-      <c r="O14" s="21"/>
+      <c r="O14" s="20"/>
       <c r="P14" s="22"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="3"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>39</v>
       </c>
@@ -1790,12 +1790,12 @@
         <v>68</v>
       </c>
       <c r="N15" s="15"/>
-      <c r="O15" s="21"/>
+      <c r="O15" s="20"/>
       <c r="P15" s="22"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>40</v>
       </c>
@@ -1829,12 +1829,12 @@
         <v>68</v>
       </c>
       <c r="N16" s="15"/>
-      <c r="O16" s="21"/>
+      <c r="O16" s="20"/>
       <c r="P16" s="22"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>41</v>
       </c>
@@ -1868,12 +1868,12 @@
         <v>68</v>
       </c>
       <c r="N17" s="15"/>
-      <c r="O17" s="21"/>
+      <c r="O17" s="20"/>
       <c r="P17" s="22"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="3"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1907,12 +1907,12 @@
         <v>68</v>
       </c>
       <c r="N18" s="15"/>
-      <c r="O18" s="21"/>
+      <c r="O18" s="20"/>
       <c r="P18" s="22"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="3"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>43</v>
       </c>
@@ -1946,12 +1946,12 @@
         <v>68</v>
       </c>
       <c r="N19" s="15"/>
-      <c r="O19" s="21"/>
+      <c r="O19" s="20"/>
       <c r="P19" s="22"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="3"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>44</v>
       </c>
@@ -1985,12 +1985,12 @@
         <v>68</v>
       </c>
       <c r="N20" s="15"/>
-      <c r="O20" s="21"/>
+      <c r="O20" s="20"/>
       <c r="P20" s="22"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="3"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>45</v>
       </c>
@@ -2024,14 +2024,14 @@
         <v>68</v>
       </c>
       <c r="N21" s="15"/>
-      <c r="O21" s="21"/>
+      <c r="O21" s="20"/>
       <c r="P21" s="22"/>
       <c r="Q21" s="6" t="s">
         <v>61</v>
       </c>
       <c r="R21" s="3"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>46</v>
       </c>
@@ -2067,12 +2067,12 @@
         <v>68</v>
       </c>
       <c r="N22" s="15"/>
-      <c r="O22" s="21"/>
+      <c r="O22" s="20"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="3"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="15"/>
       <c r="D23" s="6"/>
@@ -2086,12 +2086,12 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="15"/>
-      <c r="O23" s="21"/>
+      <c r="O23" s="20"/>
       <c r="P23" s="22"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>47</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>68</v>
       </c>
       <c r="N24" s="15"/>
-      <c r="O24" s="21"/>
+      <c r="O24" s="20"/>
       <c r="P24" s="22"/>
       <c r="Q24" s="6" t="s">
         <v>61</v>
@@ -2132,7 +2132,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="C25" s="15"/>
       <c r="D25" s="6"/>
@@ -2146,12 +2146,12 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="15"/>
-      <c r="O25" s="21"/>
+      <c r="O25" s="20"/>
       <c r="P25" s="22"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="3"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>48</v>
       </c>
@@ -2187,14 +2187,14 @@
       <c r="N26" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O26" s="21" t="s">
+      <c r="O26" s="20" t="s">
         <v>64</v>
       </c>
       <c r="P26" s="22"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="3"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>49</v>
       </c>
@@ -2230,14 +2230,14 @@
       <c r="N27" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O27" s="21" t="s">
+      <c r="O27" s="20" t="s">
         <v>64</v>
       </c>
       <c r="P27" s="22"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="3"/>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
         <v>50</v>
       </c>
@@ -2273,14 +2273,14 @@
       <c r="N28" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O28" s="21" t="s">
+      <c r="O28" s="20" t="s">
         <v>64</v>
       </c>
       <c r="P28" s="22"/>
       <c r="Q28" s="15"/>
       <c r="R28" s="3"/>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="15" t="s">
         <v>51</v>
       </c>
@@ -2316,14 +2316,14 @@
       <c r="N29" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O29" s="21" t="s">
+      <c r="O29" s="20" t="s">
         <v>65</v>
       </c>
       <c r="P29" s="22"/>
       <c r="Q29" s="15"/>
       <c r="R29" s="3"/>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -2337,12 +2337,12 @@
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
-      <c r="O30" s="21"/>
+      <c r="O30" s="20"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
     </row>
-    <row r="31" spans="2:18" ht="31" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B31" s="15" t="s">
         <v>52</v>
       </c>
@@ -2374,12 +2374,12 @@
         <v>68</v>
       </c>
       <c r="N31" s="15"/>
-      <c r="O31" s="21"/>
+      <c r="O31" s="20"/>
       <c r="P31" s="22"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="15"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2393,12 +2393,12 @@
       <c r="L32" s="2"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="21"/>
+      <c r="O32" s="20"/>
       <c r="P32" s="22"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>53</v>
       </c>
@@ -2432,12 +2432,12 @@
         <v>68</v>
       </c>
       <c r="N33" s="16"/>
-      <c r="O33" s="21"/>
+      <c r="O33" s="20"/>
       <c r="P33" s="22"/>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
     </row>
-    <row r="34" spans="2:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>22</v>
       </c>
@@ -2477,7 +2477,7 @@
       <c r="N34" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="O34" s="21" t="s">
+      <c r="O34" s="20" t="s">
         <v>64</v>
       </c>
       <c r="P34" s="22"/>
@@ -2488,14 +2488,14 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="20" t="s">
         <v>82</v>
       </c>
       <c r="E35" s="22"/>
@@ -2508,21 +2508,21 @@
       <c r="H35" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="I35" s="21" t="s">
+      <c r="I35" s="20" t="s">
         <v>84</v>
       </c>
       <c r="J35" s="22"/>
       <c r="K35" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="L35" s="21" t="s">
+      <c r="L35" s="20" t="s">
         <v>87</v>
       </c>
       <c r="M35" s="22"/>
-      <c r="N35" s="21" t="s">
+      <c r="N35" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="O35" s="23"/>
+      <c r="O35" s="21"/>
       <c r="P35" s="22"/>
       <c r="Q35" s="15" t="s">
         <v>93</v>
@@ -2531,14 +2531,14 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="20" t="s">
         <v>82</v>
       </c>
       <c r="E36" s="22"/>
@@ -2569,7 +2569,7 @@
       <c r="N36" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="O36" s="21" t="s">
+      <c r="O36" s="20" t="s">
         <v>81</v>
       </c>
       <c r="P36" s="22"/>
@@ -2580,14 +2580,14 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="20" t="s">
         <v>92</v>
       </c>
       <c r="E37" s="22"/>
@@ -2615,10 +2615,10 @@
       <c r="M37" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="N37" s="21" t="s">
+      <c r="N37" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="O37" s="23"/>
+      <c r="O37" s="21"/>
       <c r="P37" s="18"/>
       <c r="Q37" s="15" t="s">
         <v>82</v>
@@ -2627,15 +2627,47 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
     <mergeCell ref="N37:O37"/>
     <mergeCell ref="O27:P27"/>
     <mergeCell ref="O26:P26"/>
@@ -2652,38 +2684,6 @@
     <mergeCell ref="O31:P31"/>
     <mergeCell ref="O32:P32"/>
     <mergeCell ref="O33:P33"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2696,51 +2696,51 @@
   <dimension ref="B2:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.765625" customWidth="1"/>
-    <col min="2" max="2" width="7.15234375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="18.15234375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="19.84375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="18.4609375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="17.3828125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="19.4609375" style="9" customWidth="1"/>
-    <col min="8" max="8" width="13.4609375" style="9" customWidth="1"/>
-    <col min="9" max="9" width="10.84375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="15.23046875" style="9" customWidth="1"/>
-    <col min="11" max="11" width="20.765625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="18.765625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="15.23046875" style="9" customWidth="1"/>
-    <col min="14" max="14" width="15.84375" style="9" customWidth="1"/>
-    <col min="15" max="15" width="16.61328125" style="9" customWidth="1"/>
-    <col min="16" max="16" width="26.15234375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="3.75" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="19.875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="19.5" style="9" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="9" customWidth="1"/>
+    <col min="9" max="9" width="10.875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="15.25" style="9" customWidth="1"/>
+    <col min="11" max="11" width="20.75" style="9" customWidth="1"/>
+    <col min="12" max="12" width="18.75" style="9" customWidth="1"/>
+    <col min="13" max="13" width="15.25" style="9" customWidth="1"/>
+    <col min="14" max="14" width="15.875" style="9" customWidth="1"/>
+    <col min="15" max="15" width="16.625" style="9" customWidth="1"/>
+    <col min="16" max="16" width="26.125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="24"/>
       <c r="C3" s="10" t="s">
         <v>83</v>
@@ -2785,7 +2785,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>30</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>31</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>32</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>33</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>34</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>35</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>36</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>37</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
@@ -3178,7 +3178,7 @@
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
         <v>38</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>39</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>40</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>41</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
         <v>42</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
         <v>43</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
         <v>44</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
         <v>45</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
         <v>46</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -3618,7 +3618,7 @@
       <c r="O22" s="15"/>
       <c r="P22" s="6"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="15" t="s">
         <v>47</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="15"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -3682,7 +3682,7 @@
       <c r="O24" s="15"/>
       <c r="P24" s="6"/>
     </row>
-    <row r="25" spans="2:16" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
         <v>48</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="2:16" ht="31" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
         <v>49</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="2:16" ht="31" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B27" s="15" t="s">
         <v>50</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="2:16" ht="31" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
         <v>51</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="15"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -3887,7 +3887,7 @@
       <c r="O29" s="15"/>
       <c r="P29" s="6"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="15" t="s">
         <v>52</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -3951,7 +3951,7 @@
       <c r="O31" s="15"/>
       <c r="P31" s="15"/>
     </row>
-    <row r="32" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="s">
         <v>53</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>

</xml_diff>

<commit_message>
lab2-2: finish EXE & WB, left test & combination (#6)
* Update xlsx & Update all `.v` file, aka. format the code

* lab2-2: implement necessary `control.v`

* lab2-2: implement `alu.v` without test

* lab2-2: implement `comp.v` & `exe_top.v` without test

* lab2-2: update `README`

* lab2-2: finish all without test
</commit_message>
<xml_diff>
--- a/Datapath_Control_Sheet.xlsx
+++ b/Datapath_Control_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Project\iverilog\Exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE605B31-6CC1-451B-B0F2-7FE2DB189768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C2EDC6-810B-4A55-AB18-06DD7ECD777B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="180">
   <si>
     <t>所属单元</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -738,6 +738,14 @@
   </si>
   <si>
     <t>BrSel_Bge(3'b100)</t>
+  </si>
+  <si>
+    <t>ImmSel_IS(3'b110)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ImmSel_IS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1235,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1890,7 +1898,7 @@
         <v>61</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="L18" s="15" t="s">
         <v>62</v>
@@ -1929,7 +1937,7 @@
         <v>61</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="L19" s="15" t="s">
         <v>62</v>
@@ -1968,7 +1976,7 @@
         <v>61</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="L20" s="15" t="s">
         <v>62</v>
@@ -2688,7 +2696,7 @@
   <dimension ref="B2:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3372,7 +3380,7 @@
         <v>101</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>130</v>
@@ -3419,7 +3427,7 @@
         <v>101</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>131</v>
@@ -3466,7 +3474,7 @@
         <v>101</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>132</v>

</xml_diff>